<commit_message>
Add times, Round 2
</commit_message>
<xml_diff>
--- a/13/MARC/UMD_UVA.xlsx
+++ b/13/MARC/UMD_UVA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raghu\quidditch\live-stats\13\MARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285A9649-F89A-4471-BD11-C33D7F3903D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BE0368-E54A-4E4F-9723-182797F24C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="97">
   <si>
     <t>A</t>
   </si>
@@ -50,9 +52,6 @@
   </si>
   <si>
     <t>Q8</t>
-  </si>
-  <si>
-    <t>ET</t>
   </si>
   <si>
     <t>GD</t>
@@ -109,19 +108,10 @@
     <t>22,23</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>20,23</t>
   </si>
   <si>
     <t>TL</t>
-  </si>
-  <si>
-    <t>G</t>
   </si>
   <si>
     <t>RCA</t>
@@ -188,6 +178,153 @@
   </si>
   <si>
     <t>PEYTON BURROW</t>
+  </si>
+  <si>
+    <t>0026</t>
+  </si>
+  <si>
+    <t>0102</t>
+  </si>
+  <si>
+    <t>0147</t>
+  </si>
+  <si>
+    <t>0158</t>
+  </si>
+  <si>
+    <t>0253</t>
+  </si>
+  <si>
+    <t>0444</t>
+  </si>
+  <si>
+    <t>0516</t>
+  </si>
+  <si>
+    <t>0605</t>
+  </si>
+  <si>
+    <t>0638</t>
+  </si>
+  <si>
+    <t>0630</t>
+  </si>
+  <si>
+    <t>0711</t>
+  </si>
+  <si>
+    <t>0718</t>
+  </si>
+  <si>
+    <t>0747</t>
+  </si>
+  <si>
+    <t>0949</t>
+  </si>
+  <si>
+    <t>1034</t>
+  </si>
+  <si>
+    <t>1113</t>
+  </si>
+  <si>
+    <t>1122</t>
+  </si>
+  <si>
+    <t>1257</t>
+  </si>
+  <si>
+    <t>1347</t>
+  </si>
+  <si>
+    <t>1359</t>
+  </si>
+  <si>
+    <t>1441</t>
+  </si>
+  <si>
+    <t>1448</t>
+  </si>
+  <si>
+    <t>1530</t>
+  </si>
+  <si>
+    <t>1618</t>
+  </si>
+  <si>
+    <t>1704</t>
+  </si>
+  <si>
+    <t>1756</t>
+  </si>
+  <si>
+    <t>1821</t>
+  </si>
+  <si>
+    <t>1925</t>
+  </si>
+  <si>
+    <t>1950</t>
+  </si>
+  <si>
+    <t>8,9</t>
+  </si>
+  <si>
+    <t>2051</t>
+  </si>
+  <si>
+    <t>2115</t>
+  </si>
+  <si>
+    <t>2123</t>
+  </si>
+  <si>
+    <t>2148</t>
+  </si>
+  <si>
+    <t>2251</t>
+  </si>
+  <si>
+    <t>2320</t>
+  </si>
+  <si>
+    <t>JOE SCHINDERLE</t>
+  </si>
+  <si>
+    <t>EY</t>
+  </si>
+  <si>
+    <t>20,21</t>
+  </si>
+  <si>
+    <t>8,47</t>
+  </si>
+  <si>
+    <t>2454</t>
+  </si>
+  <si>
+    <t>2518</t>
+  </si>
+  <si>
+    <t>2634</t>
+  </si>
+  <si>
+    <t>2649</t>
+  </si>
+  <si>
+    <t>2743</t>
+  </si>
+  <si>
+    <t>2805</t>
+  </si>
+  <si>
+    <t>2830</t>
+  </si>
+  <si>
+    <t>2909</t>
+  </si>
+  <si>
+    <t>2758</t>
   </si>
 </sst>
 </file>
@@ -440,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -482,7 +619,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -490,17 +635,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,8 +862,8 @@
   </sheetPr>
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -751,21 +891,21 @@
     <row r="1" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
       <c r="R1" s="2"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -778,40 +918,40 @@
     </row>
     <row r="2" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="23" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="23">
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="19">
         <f>COUNTIFS(A:A,"G*") + COUNTIFS(G:G,"G*")+COUNTIFS(M:M,"G*")</f>
         <v>8</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="23" t="e">
-        <f ca="1">_xludf.TEXTJOIN("",TRUE,IF(COUNTIF($A$7:$R$32,"RCA"),"*",""),IF(COUNTIF($A$7:$R$32,"OCA"),"^",""),IF(COUNTIF($A$7:$R$32,"2CA"),"!",""))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="15" t="e">
-        <f ca="1">_xludf.CONCAT(LEN(O2)*30+L2*10,O2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="17"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="26" t="str">
+        <f>IF(COUNTIF($A$7:$R$32,"RCA"),"*","")&amp;IF(COUNTIF($A$7:$R$32,"OCA"),"^","")&amp;IF(COUNTIF($A$7:$R$32,"2CA"),"!","")</f>
+        <v>*</v>
+      </c>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="25" t="str">
+        <f>CONCATENATE(LEN(O2)*30+L2*10,O2)</f>
+        <v>110*</v>
+      </c>
+      <c r="S2" s="20"/>
+      <c r="T2" s="21"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
@@ -821,25 +961,25 @@
     </row>
     <row r="3" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="20"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="24"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
@@ -849,40 +989,40 @@
     </row>
     <row r="4" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="23" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="23">
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="19">
         <f>COUNTIFS(D:D,"G*")+COUNTIFS(J:J,"G*")+COUNTIFS(P:P,"G*")</f>
         <v>7</v>
       </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="23" t="e">
-        <f ca="1">_xludf.TEXTJOIN("",TRUE,IF(COUNTIF($A$7:$R$32,"RCB"),"*",""),IF(COUNTIF($A$7:$R$32,"OCB"),"^",""),IF(COUNTIF($A$7:$R$32,"2CB"),"!",""))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="15" t="e">
-        <f ca="1">_xludf.CONCAT(LEN(O4)*30+L4*10,O4)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="S4" s="16"/>
-      <c r="T4" s="17"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="26" t="str">
+        <f>IF(COUNTIF($A$7:$R$32,"RCB"),"*","")&amp;IF(COUNTIF($A$7:$R$32,"OCB"),"^","")&amp;IF(COUNTIF($A$7:$R$32,"2CB"),"!","")</f>
+        <v/>
+      </c>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="25" t="str">
+        <f>CONCATENATE(LEN(O4)*30+L4*10,O4)</f>
+        <v>70</v>
+      </c>
+      <c r="S4" s="20"/>
+      <c r="T4" s="21"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -892,25 +1032,25 @@
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="20"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="24"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -956,27 +1096,37 @@
       <c r="E7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="8"/>
+      <c r="L7" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="M7" s="3"/>
       <c r="N7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O7" s="5"/>
+      <c r="O7" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R7" s="8"/>
+      <c r="R7" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -991,21 +1141,23 @@
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="9" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E8" s="10">
         <v>13</v>
       </c>
-      <c r="F8" s="11"/>
+      <c r="F8" s="11">
+        <v>23</v>
+      </c>
       <c r="G8" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8" s="10">
         <v>20</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K8" s="10">
         <v>6</v>
@@ -1014,7 +1166,7 @@
         <v>9</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N8" s="10">
         <v>69</v>
@@ -1023,7 +1175,7 @@
         <v>21</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q8" s="10">
         <v>8</v>
@@ -1073,32 +1225,44 @@
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="L10" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="M10" s="3"/>
       <c r="N10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="5"/>
+      <c r="O10" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R10" s="8"/>
+      <c r="R10" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -1110,7 +1274,7 @@
     </row>
     <row r="11" spans="1:26" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="10">
         <v>46</v>
@@ -1119,7 +1283,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="10">
         <v>6</v>
@@ -1128,14 +1292,14 @@
         <v>47</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="10">
         <v>21</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K11" s="10">
         <v>26</v>
@@ -1144,14 +1308,14 @@
         <v>50</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N11" s="10">
         <v>20</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q11" s="10">
         <v>50</v>
@@ -1201,34 +1365,46 @@
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="G13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="J13" s="6"/>
       <c r="K13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O13" s="5"/>
+      <c r="O13" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R13" s="8"/>
+      <c r="R13" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
@@ -1240,7 +1416,7 @@
     </row>
     <row r="14" spans="1:26" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="10">
         <v>33</v>
@@ -1249,7 +1425,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="10">
         <v>6</v>
@@ -1258,25 +1434,25 @@
         <v>26</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" s="10">
         <v>44</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K14" s="10">
         <v>22</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N14" s="10">
         <v>69</v>
@@ -1285,13 +1461,13 @@
         <v>21</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q14" s="10">
         <v>22</v>
       </c>
       <c r="R14" s="11">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -1332,39 +1508,51 @@
     </row>
     <row r="16" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="J16" s="6"/>
       <c r="K16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L16" s="8"/>
+      <c r="L16" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="M16" s="3"/>
       <c r="N16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O16" s="5"/>
+      <c r="O16" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="P16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R16" s="8"/>
+      <c r="R16" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
@@ -1376,16 +1564,16 @@
     </row>
     <row r="17" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="13">
         <v>44</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="13">
         <v>11</v>
@@ -1394,7 +1582,7 @@
         <v>44</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H17" s="13">
         <v>22</v>
@@ -1403,7 +1591,7 @@
         <v>21</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K17" s="13">
         <v>6</v>
@@ -1412,14 +1600,14 @@
         <v>0</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N17" s="10">
         <v>20</v>
       </c>
       <c r="O17" s="11"/>
       <c r="P17" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q17" s="10">
         <v>0</v>
@@ -1467,38 +1655,50 @@
       <c r="B19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="D19" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="J19" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L19" s="8"/>
+      <c r="L19" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="M19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O19" s="5"/>
+      <c r="O19" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R19" s="8"/>
+      <c r="R19" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -1510,14 +1710,14 @@
     </row>
     <row r="20" spans="1:26" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="10">
         <v>20</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E20" s="10">
         <v>20</v>
@@ -1526,38 +1726,40 @@
         <v>28</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" s="10">
         <v>8</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="L20" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="K20" s="10">
+        <v>20</v>
+      </c>
+      <c r="L20" s="11">
+        <v>9</v>
+      </c>
       <c r="M20" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N20" s="10">
         <v>8</v>
       </c>
       <c r="O20" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P20" s="9" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="Q20" s="10">
         <v>22</v>
       </c>
-      <c r="R20" s="11">
-        <v>8</v>
+      <c r="R20" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -1601,32 +1803,44 @@
       <c r="B22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="G22" s="3"/>
       <c r="H22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="5"/>
+      <c r="I22" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="J22" s="6"/>
       <c r="K22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L22" s="8"/>
+      <c r="L22" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="M22" s="3"/>
       <c r="N22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O22" s="5"/>
+      <c r="O22" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="P22" s="6"/>
       <c r="Q22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R22" s="8"/>
+      <c r="R22" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -1638,7 +1852,7 @@
     </row>
     <row r="23" spans="1:26" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="10">
         <v>23</v>
@@ -1647,7 +1861,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E23" s="10">
         <v>14</v>
@@ -1656,14 +1870,14 @@
         <v>0</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H23" s="10">
         <v>69</v>
       </c>
       <c r="I23" s="11"/>
       <c r="J23" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K23" s="10">
         <v>8</v>
@@ -1672,14 +1886,14 @@
         <v>13</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N23" s="10">
         <v>20</v>
       </c>
       <c r="O23" s="11"/>
       <c r="P23" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q23" s="10">
         <v>47</v>
@@ -1729,32 +1943,44 @@
       <c r="B25" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="D25" s="6"/>
       <c r="E25" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="8"/>
+      <c r="F25" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="G25" s="3"/>
       <c r="H25" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I25" s="5"/>
+      <c r="I25" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="J25" s="6"/>
       <c r="K25" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L25" s="8"/>
+      <c r="L25" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="M25" s="3"/>
       <c r="N25" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O25" s="5"/>
+      <c r="O25" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R25" s="8"/>
+      <c r="R25" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
@@ -1766,7 +1992,7 @@
     </row>
     <row r="26" spans="1:26" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" s="10">
         <v>94</v>
@@ -1775,7 +2001,7 @@
         <v>20</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" s="10">
         <v>8</v>
@@ -1784,35 +2010,39 @@
         <v>13</v>
       </c>
       <c r="G26" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="10">
         <v>6</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K26" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="L26" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="K26" s="10">
+        <v>47</v>
+      </c>
+      <c r="L26" s="11">
+        <v>8</v>
+      </c>
       <c r="M26" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N26" s="10">
         <v>50</v>
       </c>
-      <c r="O26" s="11">
+      <c r="O26" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q26" s="10">
         <v>20</v>
       </c>
-      <c r="P26" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q26" s="10">
-        <v>50</v>
-      </c>
-      <c r="R26" s="11"/>
+      <c r="R26" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -1855,17 +2085,23 @@
       <c r="B28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="D28" s="6"/>
       <c r="E28" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="8"/>
+      <c r="F28" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="G28" s="3"/>
       <c r="H28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I28" s="5"/>
+      <c r="I28" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="J28" s="6"/>
       <c r="K28" s="7" t="s">
         <v>3</v>
@@ -1892,7 +2128,7 @@
     </row>
     <row r="29" spans="1:26" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" s="10">
         <v>46</v>
@@ -1901,14 +2137,14 @@
         <v>20</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E29" s="10">
         <v>47</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H29" s="10">
         <v>21</v>
@@ -29274,6 +29510,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="R2:T3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:H5"/>
+    <mergeCell ref="I4:K5"/>
+    <mergeCell ref="L4:N5"/>
+    <mergeCell ref="O4:Q5"/>
+    <mergeCell ref="R4:T5"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:N1"/>
@@ -29283,13 +29526,6 @@
     <mergeCell ref="I2:K3"/>
     <mergeCell ref="L2:N3"/>
     <mergeCell ref="O2:Q3"/>
-    <mergeCell ref="R2:T3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:H5"/>
-    <mergeCell ref="I4:K5"/>
-    <mergeCell ref="L4:N5"/>
-    <mergeCell ref="O4:Q5"/>
-    <mergeCell ref="R4:T5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -29309,8 +29545,8 @@
   </sheetPr>
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29331,7 +29567,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29364,7 +29600,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29377,7 +29613,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29385,7 +29621,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29398,7 +29634,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29411,7 +29647,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29419,7 +29655,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29452,7 +29688,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29460,7 +29696,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29468,7 +29704,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29476,10 +29712,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29507,7 +29743,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29515,7 +29751,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29538,7 +29774,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29596,7 +29832,7 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29609,7 +29845,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29617,7 +29853,7 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29635,7 +29871,7 @@
         <v>50</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29733,10 +29969,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C71" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29784,84 +30020,87 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="14">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="14">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="14">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="14">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="14">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="14">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="14">
         <v>94</v>
+      </c>
+      <c r="C96" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>